<commit_message>
Implementing NLTK for portuguese text processing.
</commit_message>
<xml_diff>
--- a/resource/model.xlsx
+++ b/resource/model.xlsx
@@ -5,23 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emanuel/Developer/md-sentiment-analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emanuel/Developer/md-sentiment-analysis/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824E7DC7-A91B-AC4B-AAE7-CF715FDFCCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238C3835-D2FB-A144-92AB-CD691B2C6F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Result 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Query" sheetId="2" r:id="rId2"/>
+    <sheet name="model" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="104">
   <si>
     <t>text</t>
   </si>
@@ -374,10 +373,6 @@
   </si>
   <si>
     <t>O cadastro dos pacientes no hospital que trabalho agora vai ter a opção de colocar nome social. Pode até parecer estranho, em 2022 isso ainda ser novidade pra alguns estabelecimentos. 🙏🙏🙏 Vitória</t>
-  </si>
-  <si>
-    <t>SELECT t.*
-FROM twitter.nome_social t</t>
   </si>
   <si>
     <t>sentiment</t>
@@ -1243,7 +1238,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1251,7 +1246,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1259,7 +1254,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1267,7 +1262,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1275,7 +1270,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1283,7 +1278,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1291,7 +1286,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1299,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1307,7 +1302,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1315,7 +1310,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1323,7 +1318,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1331,7 +1326,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1339,7 +1334,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1347,7 +1342,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1355,7 +1350,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1363,7 +1358,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1371,7 +1366,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1379,7 +1374,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1387,7 +1382,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1395,7 +1390,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1403,7 +1398,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1411,7 +1406,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1419,7 +1414,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1427,7 +1422,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1435,7 +1430,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1443,7 +1438,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1451,7 +1446,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1459,7 +1454,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1467,7 +1462,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1475,7 +1470,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1483,7 +1478,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1491,7 +1486,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1499,7 +1494,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1507,7 +1502,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1515,7 +1510,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1523,7 +1518,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1531,7 +1526,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1539,7 +1534,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1547,7 +1542,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1555,7 +1550,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1563,7 +1558,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -1571,7 +1566,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1579,7 +1574,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -1587,7 +1582,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -1595,7 +1590,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1603,7 +1598,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1611,7 +1606,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1619,7 +1614,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1627,7 +1622,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1635,7 +1630,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1643,7 +1638,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1651,7 +1646,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1659,7 +1654,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1667,7 +1662,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1675,7 +1670,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1683,7 +1678,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -1691,7 +1686,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1699,7 +1694,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1707,7 +1702,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1715,7 +1710,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -1723,7 +1718,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -1731,7 +1726,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -1739,7 +1734,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -1747,7 +1742,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -1755,7 +1750,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -1763,7 +1758,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -1771,7 +1766,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -1779,7 +1774,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -1787,7 +1782,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -1795,7 +1790,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -1803,7 +1798,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -1811,7 +1806,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -1819,7 +1814,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -1827,7 +1822,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -1835,7 +1830,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -1843,7 +1838,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -1851,7 +1846,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -1859,7 +1854,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -1867,7 +1862,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -1875,7 +1870,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -1883,7 +1878,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -1891,7 +1886,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -1899,7 +1894,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -1907,7 +1902,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -1915,7 +1910,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -1923,7 +1918,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -1931,7 +1926,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
@@ -1939,7 +1934,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -1947,7 +1942,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
@@ -1955,7 +1950,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
@@ -1963,7 +1958,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
@@ -1971,7 +1966,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -1979,7 +1974,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
@@ -1987,7 +1982,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -1995,7 +1990,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -2003,7 +1998,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -2011,7 +2006,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -2019,7 +2014,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -2027,7 +2022,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -2035,7 +2030,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -2043,25 +2038,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>104</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>